<commit_message>
Added DDT test for cucumber
</commit_message>
<xml_diff>
--- a/testData/LetsShop_LoginData.xlsx
+++ b/testData/LetsShop_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusch\eclipse-workspace\LetsShopV26\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC11438-6EB2-45AB-BA39-A193AB6C4F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691FB413-BA7A-4BEE-92E9-ADD9BB2FDBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -36,15 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>res</t>
-  </si>
-  <si>
     <t>lakshmi@yahoo.com</t>
   </si>
   <si>
@@ -79,13 +70,22 @@
   </si>
   <si>
     <t>Test@12345</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,19 +124,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -169,9 +171,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -180,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -499,7 +501,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,70 +511,70 @@
     <col min="3" max="3" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>